<commit_message>
Binary Search Tree-LC and GFG
LC-144,145,700,701,94
GFG-216
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Binary Search Tree\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5E4005-5D94-4253-92BA-614AD38203D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+  <si>
+    <t>Question No</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>GFG/LC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Binary Tree Inorder Traversal(Inorder Tree Traversal -Recursive)</t>
+  </si>
+  <si>
+    <t>Insert into a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Search in a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>GFG</t>
+  </si>
+  <si>
+    <t>Minimum element in BST (Find min and max value in a BST)</t>
+  </si>
+  <si>
+    <t>Binary Tree Postorder Traversal-Recursive</t>
+  </si>
+  <si>
+    <t>Binary Tree Preorder Traversal-Recursive</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +101,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +391,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>145</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>701</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>700</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>216</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
938-GFG-Range sum in BST
938-GFG-Range sum in BST
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5E4005-5D94-4253-92BA-614AD38203D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE50E442-48D9-449B-B8D5-8DCF7C6D702D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Question No</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Binary Tree Preorder Traversal-Recursive</t>
+  </si>
+  <si>
+    <t>LC/GFG</t>
+  </si>
+  <si>
+    <t>Count BST nodes that lie in a given range</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +486,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>938</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
104-GFG-Maximum Depth of Binary Tree or Height of Binary Tree
104-GFG-Maximum Depth of Binary Tree or Height of Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Binary Search Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE50E442-48D9-449B-B8D5-8DCF7C6D702D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9BAB9-BDDB-4613-8608-DF1346FEF24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Question No</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Count BST nodes that lie in a given range</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree or Height of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +500,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Top view of Binary Tree
GFG-Top view of Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9BAB9-BDDB-4613-8608-DF1346FEF24B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D7F2F-2707-457C-83FD-5631F1EAB0A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Question No</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Maximum Depth of Binary Tree or Height of Binary Tree</t>
+  </si>
+  <si>
+    <t>Top View of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +514,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Top view, bottom view of binary tree
1. Top view of binary tree-Updated code.
2. Bottom view of binary tree.
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0230CA11-96AD-478C-9178-5F6738976D1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385ADAA-FE7C-4065-8A2B-316975D1E4E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Question No</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Binary Tree Zigzag Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Bottom View of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +661,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
236-GFG-Find LCA in a Binary Tree
236-GFG-Find LCA in a Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385ADAA-FE7C-4065-8A2B-316975D1E4E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3E406A-08C9-4420-8688-AD0FFA3823C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Question No</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Bottom View of Binary Tree</t>
+  </si>
+  <si>
+    <t>Find LCA in a Binary tree</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="A20:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +675,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>236</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
662.Maximum Width of Binary tree
662.Maximum Width of Binary tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3E406A-08C9-4420-8688-AD0FFA3823C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE25E65-9441-4777-8EED-5074FAD98BEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>Question No</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Find LCA in a Binary tree</t>
+  </si>
+  <si>
+    <t>Maximum Width of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,6 +689,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>662</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Transform to Sum Tree
GFG-Transform to Sum Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484376E5-2C11-44D5-85D3-79BCBEF60AD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EC922-E6DE-4121-9C9B-195578E521F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>Question No</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Transform to Sum Tree</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,6 +735,17 @@
       </c>
       <c r="D23" s="6"/>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Diagonal Traversal of Binary tree
GFG-Diagonal Traversal of Binary tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EC922-E6DE-4121-9C9B-195578E521F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E032EF18-227E-4B07-BF73-D62551DAE0E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Question No</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Transform to Sum Tree</t>
+  </si>
+  <si>
+    <t>Diagonal Traversal of Binary Tree </t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,6 +749,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
226-GFG-Invert Binary tree (Mirror image of tree)
226-GFG-Invert Binary tree (Mirror image of tree)
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E032EF18-227E-4B07-BF73-D62551DAE0E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169ED4CC-4BF4-4159-8DF9-96810A89FF06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Question No</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Diagonal Traversal of Binary Tree </t>
+  </si>
+  <si>
+    <t>Invert Binary Tree(Mirror Tree)</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +763,17 @@
         <v>30</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>226</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
297.Serialize and Deserialize Binary Tree
297.Serialize and Deserialize Binary Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169ED4CC-4BF4-4159-8DF9-96810A89FF06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108CC556-A009-4DAD-B414-7842CB2B6420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Question No</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Invert Binary Tree(Mirror Tree)</t>
+  </si>
+  <si>
+    <t>Serialize and Deserialize Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +777,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>297</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Before going on a break
Before going on a break
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB9CFE-076F-411F-BA0A-0978CFBD33D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC39351-24C0-4C49-A9CC-B30084C3DE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Question No</t>
   </si>
@@ -130,6 +130,30 @@
   </si>
   <si>
     <t>Count Complete Tree Nodes</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Inorder and Postorder Traversal</t>
+  </si>
+  <si>
+    <t>Morris Traversal</t>
+  </si>
+  <si>
+    <t>Morris Traversal-Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>Morriss</t>
+  </si>
+  <si>
+    <t>Morris Traversal-Binary Tree Preorder Traversal</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>Recursion</t>
   </si>
 </sst>
 </file>
@@ -484,16 +508,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -816,6 +841,84 @@
         <v>34</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>106</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>235</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>114</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>114</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG and codestudio problem
1. GFG-Find the closest element in BST
2. Floor and Ceil in BST
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC39351-24C0-4C49-A9CC-B30084C3DE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B5DFF7-E8E8-41AE-AEA9-96E1FADD4F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Question No</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Recursion</t>
+  </si>
+  <si>
+    <t>Find the Closest Element in BST</t>
+  </si>
+  <si>
+    <t>Floor  and Ceil in BST.py</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,6 +925,28 @@
         <v>42</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
450.Delete a Node from tree
450.Delete a Node from tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B5DFF7-E8E8-41AE-AEA9-96E1FADD4F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF0568D-E6FE-41F6-BBF3-E75B6A79630E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Question No</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Floor  and Ceil in BST.py</t>
+  </si>
+  <si>
+    <t>Delete Node in a BST</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
@@ -947,6 +950,17 @@
         <v>44</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>450</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
98-GFG.Validate Binary Search Tree
98-GFG.Validate Binary Search Tree
</commit_message>
<xml_diff>
--- a/Binary Search Tree/Question_List.xlsx
+++ b/Binary Search Tree/Question_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Binary Search Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF0568D-E6FE-41F6-BBF3-E75B6A79630E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8078F1C-D857-4D1E-B9D2-1A3792F733CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>Question No</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Delete Node in a BST</t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,6 +964,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>